<commit_message>
fixes, implement feature stacking classifier
</commit_message>
<xml_diff>
--- a/results/fn.xlsx
+++ b/results/fn.xlsx
@@ -362,7 +362,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q26"/>
+  <dimension ref="A1:Q21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -531,7 +531,7 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>3214</v>
+        <v>3205</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -566,16 +566,16 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>ja ampak zakaj noče</t>
+          <t>zakaj mu pehta preprosto ne da</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>Yes but why doesn't she want to?</t>
+          <t>Why can't Pehta just give it to him?</t>
         </is>
       </c>
       <c r="K3" s="2" t="n">
-        <v>43536.26611111111</v>
+        <v>43536.26012731482</v>
       </c>
       <c r="L3" t="inlineStr">
         <is>
@@ -583,7 +583,7 @@
         </is>
       </c>
       <c r="M3" t="n">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="N3" t="inlineStr">
         <is>
@@ -608,7 +608,7 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>3216</v>
+        <v>3231</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -625,7 +625,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Kako pa bi se ti počutil/-a, če bi moral/-a zapustiti svojo družino? Zakaj? / How would you feel if you had to leave your family? Why?</t>
+          <t>Mojca je bila prepričana, da je z njo ženska iz vasi. Ali misliš, da bi drugače vseeno odšla s Pehto? Zakaj? / Mojca was sure, that the woman she met was someone from the village. Do you think she would still leave with Pehta if she thought otherwise? Why?</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -643,16 +643,16 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>jaz se bi počuz</t>
+          <t>aja</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>I would feel (there is a typo, no further answer provided)</t>
+          <t>Oh</t>
         </is>
       </c>
       <c r="K4" s="2" t="n">
-        <v>43536.23444444445</v>
+        <v>43536.24097222222</v>
       </c>
       <c r="L4" t="inlineStr">
         <is>
@@ -660,7 +660,7 @@
         </is>
       </c>
       <c r="M4" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="N4" t="inlineStr">
         <is>
@@ -674,7 +674,7 @@
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>DA</t>
+          <t>DAA</t>
         </is>
       </c>
       <c r="Q4" t="inlineStr">
@@ -685,7 +685,7 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>3231</v>
+        <v>3233</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -729,7 +729,7 @@
         </is>
       </c>
       <c r="K5" s="2" t="n">
-        <v>43536.24097222222</v>
+        <v>43536.24106481481</v>
       </c>
       <c r="L5" t="inlineStr">
         <is>
@@ -762,7 +762,7 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>3233</v>
+        <v>3239</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -788,25 +788,25 @@
         </is>
       </c>
       <c r="G6" t="n">
-        <v>718</v>
+        <v>720</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>filipkrstic</t>
+          <t>tijanamiljanovic</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>aja</t>
+          <t>jp</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>Oh</t>
+          <t>Yep</t>
         </is>
       </c>
       <c r="K6" s="2" t="n">
-        <v>43536.24106481481</v>
+        <v>43536.24672453704</v>
       </c>
       <c r="L6" t="inlineStr">
         <is>
@@ -814,7 +814,7 @@
         </is>
       </c>
       <c r="M6" t="n">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="N6" t="inlineStr">
         <is>
@@ -828,7 +828,7 @@
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>DAA</t>
+          <t>DA</t>
         </is>
       </c>
       <c r="Q6" t="inlineStr">
@@ -839,7 +839,7 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>3239</v>
+        <v>3241</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -874,16 +874,16 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>jp</t>
+          <t>jaz pa ne zakaj</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>Yep</t>
+          <t>I wouldn't want to be him. Why (would you want to be him)?</t>
         </is>
       </c>
       <c r="K7" s="2" t="n">
-        <v>43536.24672453704</v>
+        <v>43536.25361111111</v>
       </c>
       <c r="L7" t="inlineStr">
         <is>
@@ -891,7 +891,7 @@
         </is>
       </c>
       <c r="M7" t="n">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="N7" t="inlineStr">
         <is>
@@ -900,12 +900,12 @@
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>Q</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>DA</t>
+          <t>DQ</t>
         </is>
       </c>
       <c r="Q7" t="inlineStr">
@@ -916,7 +916,7 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>3241</v>
+        <v>3242</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -942,25 +942,25 @@
         </is>
       </c>
       <c r="G8" t="n">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>tijanamiljanovic</t>
+          <t>filipkrstic</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>jaz pa ne zakaj</t>
+          <t>hecam se mojca</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>I wouldn't want to be him. Why (would you want to be him)?</t>
+          <t>I'm kidding, (I'd want to be) Mojca</t>
         </is>
       </c>
       <c r="K8" s="2" t="n">
-        <v>43536.25361111111</v>
+        <v>43536.25422453704</v>
       </c>
       <c r="L8" t="inlineStr">
         <is>
@@ -968,7 +968,7 @@
         </is>
       </c>
       <c r="M8" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N8" t="inlineStr">
         <is>
@@ -977,12 +977,12 @@
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>Q</t>
+          <t>A</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t>DQ</t>
+          <t>DAA</t>
         </is>
       </c>
       <c r="Q8" t="inlineStr">
@@ -993,7 +993,7 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>3242</v>
+        <v>3245</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -1019,25 +1019,25 @@
         </is>
       </c>
       <c r="G9" t="n">
-        <v>718</v>
+        <v>720</v>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>filipkrstic</t>
+          <t>tijanamiljanovic</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>hecam se mojca</t>
+          <t>oprosti mojca</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>I'm kidding, (I'd want to be) Mojca</t>
+          <t>I'm sorry Mojca</t>
         </is>
       </c>
       <c r="K9" s="2" t="n">
-        <v>43536.25422453704</v>
+        <v>43536.25638888889</v>
       </c>
       <c r="L9" t="inlineStr">
         <is>
@@ -1045,7 +1045,7 @@
         </is>
       </c>
       <c r="M9" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="N9" t="inlineStr">
         <is>
@@ -1070,7 +1070,7 @@
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>3245</v>
+        <v>3263</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -1092,29 +1092,29 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Knjižni Klub 7</t>
+          <t>Knjižni Klub 8</t>
         </is>
       </c>
       <c r="G10" t="n">
-        <v>720</v>
+        <v>676</v>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>tijanamiljanovic</t>
+          <t>karin japelj K</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>oprosti mojca</t>
+          <t>itak</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>I'm sorry Mojca</t>
+          <t xml:space="preserve">Of course. </t>
         </is>
       </c>
       <c r="K10" s="2" t="n">
-        <v>43536.25638888889</v>
+        <v>43536.26666666667</v>
       </c>
       <c r="L10" t="inlineStr">
         <is>
@@ -1122,7 +1122,7 @@
         </is>
       </c>
       <c r="M10" t="n">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="N10" t="inlineStr">
         <is>
@@ -1136,7 +1136,7 @@
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>DAA</t>
+          <t>DA</t>
         </is>
       </c>
       <c r="Q10" t="inlineStr">
@@ -1147,51 +1147,51 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>3253</v>
+        <v>3312</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>OŠ Koseze</t>
+          <t>OŠ Šmartno pod Šmarno goro</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Koseze</t>
+          <t>Smartno</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Kako pa bi se ti počutil/-a, če bi moral/-a zapustiti svojo družino? Zakaj? / How would you feel if you had to leave your family? Why?</t>
+          <t>Zakaj je Replja rekla Puhanki, da ni ravno ena najpametnejših? / Why did Replja say that Puhanka is "Not one of the smartest ones"?</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Knjižni Klub 8</t>
+          <t>Book Club Three</t>
         </is>
       </c>
       <c r="G11" t="n">
-        <v>726</v>
+        <v>781</v>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>timskander</t>
+          <t>smartno8</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>prestrašeno</t>
+          <t>enako</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>scared</t>
+          <t>Same</t>
         </is>
       </c>
       <c r="K11" s="2" t="n">
-        <v>43536.23680555556</v>
+        <v>43574.14583333334</v>
       </c>
       <c r="L11" t="inlineStr">
         <is>
@@ -1199,7 +1199,7 @@
         </is>
       </c>
       <c r="M11" t="n">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="N11" t="inlineStr">
         <is>
@@ -1208,12 +1208,12 @@
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>S</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>DA</t>
+          <t>DAA</t>
         </is>
       </c>
       <c r="Q11" t="inlineStr">
@@ -1224,51 +1224,51 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>3263</v>
+        <v>3330</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>OŠ Koseze</t>
+          <t>OŠ Šmartno pod Šmarno goro</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Koseze</t>
+          <t>Smartno</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Mojca je bila prepričana, da je z njo ženska iz vasi. Ali misliš, da bi drugače vseeno odšla s Pehto? Zakaj? / Mojca was sure, that the woman she met was someone from the village. Do you think she would still leave with Pehta if she thought otherwise? Why?</t>
+          <t>Zakaj je Replja rekla Puhanki, da ni ravno ena najpametnejših? / Why did Replja say that Puhanka is "Not one of the smartest ones"?</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Knjižni Klub 8</t>
+          <t>Book Club Four</t>
         </is>
       </c>
       <c r="G12" t="n">
-        <v>676</v>
+        <v>784</v>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>karin japelj K</t>
+          <t>smartno11</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>itak</t>
+          <t>ubistvu nevem ravno</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t xml:space="preserve">Of course. </t>
+          <t>Actually I don't really know</t>
         </is>
       </c>
       <c r="K12" s="2" t="n">
-        <v>43536.26666666667</v>
+        <v>43574.15694444445</v>
       </c>
       <c r="L12" t="inlineStr">
         <is>
@@ -1276,7 +1276,7 @@
         </is>
       </c>
       <c r="M12" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="N12" t="inlineStr">
         <is>
@@ -1285,12 +1285,12 @@
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>S</t>
         </is>
       </c>
       <c r="P12" t="inlineStr">
         <is>
-          <t>DA</t>
+          <t>DAA</t>
         </is>
       </c>
       <c r="Q12" t="inlineStr">
@@ -1301,7 +1301,7 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>3273</v>
+        <v>3334</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -1314,47 +1314,47 @@
         </is>
       </c>
       <c r="D13" t="n">
+        <v>7</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Kako bi lahko Cefizelj pobegnil policistu še na drugačen način? / In what other way could Cefizelj get away from the policeman?</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Book Club One</t>
+        </is>
+      </c>
+      <c r="G13" t="n">
+        <v>793</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>smartno20</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>nevem</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>I don't know</t>
+        </is>
+      </c>
+      <c r="K13" s="2" t="n">
+        <v>43574.13263888889</v>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="M13" t="n">
         <v>5</v>
       </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>Kako bi Kekec na drugačen način prišel do zdravila? / In what other way could Kekec get the medicine?</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>Book Club One</t>
-        </is>
-      </c>
-      <c r="G13" t="n">
-        <v>785</v>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>smartno12</t>
-        </is>
-      </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>maš ti kakšno idejo?</t>
-        </is>
-      </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>Do you have any ideas?</t>
-        </is>
-      </c>
-      <c r="K13" s="2" t="n">
-        <v>43574.16041666667</v>
-      </c>
-      <c r="L13" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="M13" t="n">
-        <v>17</v>
-      </c>
       <c r="N13" t="inlineStr">
         <is>
           <t>Yes</t>
@@ -1362,7 +1362,7 @@
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>Q</t>
+          <t>A</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
@@ -1378,7 +1378,7 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>3275</v>
+        <v>3335</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
@@ -1391,47 +1391,47 @@
         </is>
       </c>
       <c r="D14" t="n">
+        <v>7</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Kako bi lahko Cefizelj pobegnil policistu še na drugačen način? / In what other way could Cefizelj get away from the policeman?</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Book Club One</t>
+        </is>
+      </c>
+      <c r="G14" t="n">
+        <v>785</v>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>smartno12</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>mmmm NEVEMM</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>mmmmm I DON'T KNOW</t>
+        </is>
+      </c>
+      <c r="K14" s="2" t="n">
+        <v>43574.13611111111</v>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="M14" t="n">
         <v>5</v>
       </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>Kako bi Kekec na drugačen način prišel do zdravila? / In what other way could Kekec get the medicine?</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>Book Club One</t>
-        </is>
-      </c>
-      <c r="G14" t="n">
-        <v>796</v>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>smartno23</t>
-        </is>
-      </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>Z čem že</t>
-        </is>
-      </c>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>With what</t>
-        </is>
-      </c>
-      <c r="K14" s="2" t="n">
-        <v>43574.16111111111</v>
-      </c>
-      <c r="L14" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="M14" t="n">
-        <v>17</v>
-      </c>
       <c r="N14" t="inlineStr">
         <is>
           <t>Yes</t>
@@ -1439,23 +1439,23 @@
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>Q</t>
+          <t>S</t>
         </is>
       </c>
       <c r="P14" t="inlineStr">
         <is>
-          <t>CO</t>
+          <t>DA</t>
         </is>
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>D</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>3278</v>
+        <v>3343</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
@@ -1468,47 +1468,47 @@
         </is>
       </c>
       <c r="D15" t="n">
+        <v>7</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Kako bi lahko Cefizelj pobegnil policistu še na drugačen način? / In what other way could Cefizelj get away from the policeman?</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Book Club Two</t>
+        </is>
+      </c>
+      <c r="G15" t="n">
+        <v>794</v>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>smartno21</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>kam</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>Where</t>
+        </is>
+      </c>
+      <c r="K15" s="2" t="n">
+        <v>43574.14652777778</v>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="M15" t="n">
         <v>5</v>
       </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>Kako bi Kekec na drugačen način prišel do zdravila? / In what other way could Kekec get the medicine?</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>Book Club One</t>
-        </is>
-      </c>
-      <c r="G15" t="n">
-        <v>785</v>
-      </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>smartno12</t>
-        </is>
-      </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>joj nevem  no ja ubistvu vem</t>
-        </is>
-      </c>
-      <c r="J15" t="inlineStr">
-        <is>
-          <t>Well I don't know well actually I do</t>
-        </is>
-      </c>
-      <c r="K15" s="2" t="n">
-        <v>43574.16180555556</v>
-      </c>
-      <c r="L15" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="M15" t="n">
-        <v>17</v>
-      </c>
       <c r="N15" t="inlineStr">
         <is>
           <t>Yes</t>
@@ -1516,23 +1516,23 @@
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>Q</t>
         </is>
       </c>
       <c r="P15" t="inlineStr">
         <is>
-          <t>CO</t>
+          <t>DQ</t>
         </is>
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>D</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>3307</v>
+        <v>3376</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
@@ -1545,47 +1545,47 @@
         </is>
       </c>
       <c r="D16" t="n">
+        <v>8</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Kaj pa bi lahko v tvojem kraju naredili, da bi bilo manj takšnih otrok, ki nimajo kaj obleči? / What could your community do to make sure there were less kids with nothing to wear?</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Book Club One</t>
+        </is>
+      </c>
+      <c r="G16" t="n">
+        <v>793</v>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>smartno20</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>jaz isto</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>Me too</t>
+        </is>
+      </c>
+      <c r="K16" s="2" t="n">
+        <v>43574.12361111111</v>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="M16" t="n">
         <v>6</v>
       </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>Zakaj je Replja rekla Puhanki, da ni ravno ena najpametnejših? / Why did Replja say that Puhanka is "Not one of the smartest ones"?</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>Book Club Two</t>
-        </is>
-      </c>
-      <c r="G16" t="n">
-        <v>794</v>
-      </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>smartno21</t>
-        </is>
-      </c>
-      <c r="I16" t="inlineStr">
-        <is>
-          <t>mama se je razjezila</t>
-        </is>
-      </c>
-      <c r="J16" t="inlineStr">
-        <is>
-          <t xml:space="preserve">mom was angry </t>
-        </is>
-      </c>
-      <c r="K16" s="2" t="n">
-        <v>43574.15902777778</v>
-      </c>
-      <c r="L16" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="M16" t="n">
-        <v>10</v>
-      </c>
       <c r="N16" t="inlineStr">
         <is>
           <t>Yes</t>
@@ -1598,7 +1598,7 @@
       </c>
       <c r="P16" t="inlineStr">
         <is>
-          <t>DA</t>
+          <t>DAA</t>
         </is>
       </c>
       <c r="Q16" t="inlineStr">
@@ -1609,7 +1609,7 @@
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>3329</v>
+        <v>3377</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
@@ -1622,38 +1622,38 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Zakaj je Replja rekla Puhanki, da ni ravno ena najpametnejših? / Why did Replja say that Puhanka is "Not one of the smartest ones"?</t>
+          <t>Kaj pa bi lahko v tvojem kraju naredili, da bi bilo manj takšnih otrok, ki nimajo kaj obleči? / What could your community do to make sure there were less kids with nothing to wear?</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Book Club Four</t>
+          <t>Book Club One</t>
         </is>
       </c>
       <c r="G17" t="n">
-        <v>784</v>
+        <v>796</v>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>smartno11</t>
+          <t>smartno23</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>ja verjetno res</t>
+          <t>zakaj že</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>Yes you are probably right</t>
+          <t xml:space="preserve">Why would you </t>
         </is>
       </c>
       <c r="K17" s="2" t="n">
-        <v>43574.15416666667</v>
+        <v>43574.125</v>
       </c>
       <c r="L17" t="inlineStr">
         <is>
@@ -1661,7 +1661,7 @@
         </is>
       </c>
       <c r="M17" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="N17" t="inlineStr">
         <is>
@@ -1670,12 +1670,12 @@
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>Q</t>
         </is>
       </c>
       <c r="P17" t="inlineStr">
         <is>
-          <t>DAA</t>
+          <t>DQ</t>
         </is>
       </c>
       <c r="Q17" t="inlineStr">
@@ -1686,7 +1686,7 @@
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>3330</v>
+        <v>3408</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
@@ -1699,47 +1699,47 @@
         </is>
       </c>
       <c r="D18" t="n">
+        <v>8</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Kaj pa bi lahko v tvojem kraju naredili, da bi bilo manj takšnih otrok, ki nimajo kaj obleči? / What could your community do to make sure there were less kids with nothing to wear?</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Book Club Three</t>
+        </is>
+      </c>
+      <c r="G18" t="n">
+        <v>782</v>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>smartno9</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>RAZDAL</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>GIVE AWAY</t>
+        </is>
+      </c>
+      <c r="K18" s="2" t="n">
+        <v>43574.12916666667</v>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="M18" t="n">
         <v>6</v>
       </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>Zakaj je Replja rekla Puhanki, da ni ravno ena najpametnejših? / Why did Replja say that Puhanka is "Not one of the smartest ones"?</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>Book Club Four</t>
-        </is>
-      </c>
-      <c r="G18" t="n">
-        <v>784</v>
-      </c>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>smartno11</t>
-        </is>
-      </c>
-      <c r="I18" t="inlineStr">
-        <is>
-          <t>ubistvu nevem ravno</t>
-        </is>
-      </c>
-      <c r="J18" t="inlineStr">
-        <is>
-          <t>Actually I don't really know</t>
-        </is>
-      </c>
-      <c r="K18" s="2" t="n">
-        <v>43574.15694444445</v>
-      </c>
-      <c r="L18" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="M18" t="n">
-        <v>15</v>
-      </c>
       <c r="N18" t="inlineStr">
         <is>
           <t>Yes</t>
@@ -1747,12 +1747,12 @@
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>A</t>
         </is>
       </c>
       <c r="P18" t="inlineStr">
         <is>
-          <t>DAA</t>
+          <t>DA</t>
         </is>
       </c>
       <c r="Q18" t="inlineStr">
@@ -1763,7 +1763,7 @@
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>3335</v>
+        <v>3453</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
@@ -1772,15 +1772,15 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Smartno</t>
+          <t>smartnoB</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Kako bi lahko Cefizelj pobegnil policistu še na drugačen način? / In what other way could Cefizelj get away from the policeman?</t>
+          <t>Zakaj je Replja rekla Puhanki, da ni ravno ena najpametnejših? / Why did Replja say that Puhanka is "Not one of the smartest ones"?</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1789,25 +1789,25 @@
         </is>
       </c>
       <c r="G19" t="n">
-        <v>785</v>
+        <v>816</v>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>smartno12</t>
+          <t>smartnoB12</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>mmmm NEVEMM</t>
+          <t>Nevem</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>mmmmm I DON'T KNOW</t>
+          <t>I don't know</t>
         </is>
       </c>
       <c r="K19" s="2" t="n">
-        <v>43574.13611111111</v>
+        <v>43581.15891203703</v>
       </c>
       <c r="L19" t="inlineStr">
         <is>
@@ -1815,7 +1815,7 @@
         </is>
       </c>
       <c r="M19" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="N19" t="inlineStr">
         <is>
@@ -1824,7 +1824,7 @@
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>A</t>
         </is>
       </c>
       <c r="P19" t="inlineStr">
@@ -1840,7 +1840,7 @@
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>3343</v>
+        <v>3460</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
@@ -1849,15 +1849,15 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Smartno</t>
+          <t>smartnoB</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Kako bi lahko Cefizelj pobegnil policistu še na drugačen način? / In what other way could Cefizelj get away from the policeman?</t>
+          <t>Zakaj je Replja rekla Puhanki, da ni ravno ena najpametnejših? / Why did Replja say that Puhanka is "Not one of the smartest ones"?</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1866,25 +1866,25 @@
         </is>
       </c>
       <c r="G20" t="n">
-        <v>794</v>
+        <v>824</v>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>smartno21</t>
+          <t>smartnoB20</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>kam</t>
+          <t>MMMMMMMMMMMMMMMMM NE VEM</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>Where</t>
+          <t>MMMMMMMMMMMMMMM I DON'T KNOW</t>
         </is>
       </c>
       <c r="K20" s="2" t="n">
-        <v>43574.14652777778</v>
+        <v>43581.14689814814</v>
       </c>
       <c r="L20" t="inlineStr">
         <is>
@@ -1892,7 +1892,7 @@
         </is>
       </c>
       <c r="M20" t="n">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="N20" t="inlineStr">
         <is>
@@ -1901,12 +1901,12 @@
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>Q</t>
+          <t>A</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
         <is>
-          <t>DQ</t>
+          <t>DA</t>
         </is>
       </c>
       <c r="Q20" t="inlineStr">
@@ -1917,7 +1917,7 @@
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>3376</v>
+        <v>3506</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
@@ -1926,7 +1926,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Smartno</t>
+          <t>smartnoB</t>
         </is>
       </c>
       <c r="D21" t="n">
@@ -1943,25 +1943,25 @@
         </is>
       </c>
       <c r="G21" t="n">
-        <v>793</v>
+        <v>823</v>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>smartno20</t>
+          <t>smartnoB19</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>jaz isto</t>
+          <t>Ja jaz sem punca</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>Me too</t>
+          <t>Yes I am a girl</t>
         </is>
       </c>
       <c r="K21" s="2" t="n">
-        <v>43574.12361111111</v>
+        <v>43581.12827546296</v>
       </c>
       <c r="L21" t="inlineStr">
         <is>
@@ -1983,395 +1983,10 @@
       </c>
       <c r="P21" t="inlineStr">
         <is>
-          <t>DAA</t>
+          <t>CO</t>
         </is>
       </c>
       <c r="Q21" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="1" t="n">
-        <v>3377</v>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>OŠ Šmartno pod Šmarno goro</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>Smartno</t>
-        </is>
-      </c>
-      <c r="D22" t="n">
-        <v>8</v>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>Kaj pa bi lahko v tvojem kraju naredili, da bi bilo manj takšnih otrok, ki nimajo kaj obleči? / What could your community do to make sure there were less kids with nothing to wear?</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>Book Club One</t>
-        </is>
-      </c>
-      <c r="G22" t="n">
-        <v>796</v>
-      </c>
-      <c r="H22" t="inlineStr">
-        <is>
-          <t>smartno23</t>
-        </is>
-      </c>
-      <c r="I22" t="inlineStr">
-        <is>
-          <t>zakaj že</t>
-        </is>
-      </c>
-      <c r="J22" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Why would you </t>
-        </is>
-      </c>
-      <c r="K22" s="2" t="n">
-        <v>43574.125</v>
-      </c>
-      <c r="L22" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="M22" t="n">
-        <v>7</v>
-      </c>
-      <c r="N22" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="O22" t="inlineStr">
-        <is>
-          <t>Q</t>
-        </is>
-      </c>
-      <c r="P22" t="inlineStr">
-        <is>
-          <t>DQ</t>
-        </is>
-      </c>
-      <c r="Q22" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="1" t="n">
-        <v>3408</v>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>OŠ Šmartno pod Šmarno goro</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>Smartno</t>
-        </is>
-      </c>
-      <c r="D23" t="n">
-        <v>8</v>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>Kaj pa bi lahko v tvojem kraju naredili, da bi bilo manj takšnih otrok, ki nimajo kaj obleči? / What could your community do to make sure there were less kids with nothing to wear?</t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>Book Club Three</t>
-        </is>
-      </c>
-      <c r="G23" t="n">
-        <v>782</v>
-      </c>
-      <c r="H23" t="inlineStr">
-        <is>
-          <t>smartno9</t>
-        </is>
-      </c>
-      <c r="I23" t="inlineStr">
-        <is>
-          <t>RAZDAL</t>
-        </is>
-      </c>
-      <c r="J23" t="inlineStr">
-        <is>
-          <t>GIVE AWAY</t>
-        </is>
-      </c>
-      <c r="K23" s="2" t="n">
-        <v>43574.12916666667</v>
-      </c>
-      <c r="L23" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="M23" t="n">
-        <v>6</v>
-      </c>
-      <c r="N23" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="O23" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="P23" t="inlineStr">
-        <is>
-          <t>DA</t>
-        </is>
-      </c>
-      <c r="Q23" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="1" t="n">
-        <v>3453</v>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>OŠ Šmartno pod Šmarno goro</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>smartnoB</t>
-        </is>
-      </c>
-      <c r="D24" t="n">
-        <v>6</v>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>Zakaj je Replja rekla Puhanki, da ni ravno ena najpametnejših? / Why did Replja say that Puhanka is "Not one of the smartest ones"?</t>
-        </is>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>Book Club One</t>
-        </is>
-      </c>
-      <c r="G24" t="n">
-        <v>816</v>
-      </c>
-      <c r="H24" t="inlineStr">
-        <is>
-          <t>smartnoB12</t>
-        </is>
-      </c>
-      <c r="I24" t="inlineStr">
-        <is>
-          <t>Nevem</t>
-        </is>
-      </c>
-      <c r="J24" t="inlineStr">
-        <is>
-          <t>I don't know</t>
-        </is>
-      </c>
-      <c r="K24" s="2" t="n">
-        <v>43581.15891203703</v>
-      </c>
-      <c r="L24" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="M24" t="n">
-        <v>10</v>
-      </c>
-      <c r="N24" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="O24" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="P24" t="inlineStr">
-        <is>
-          <t>DA</t>
-        </is>
-      </c>
-      <c r="Q24" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="1" t="n">
-        <v>3460</v>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>OŠ Šmartno pod Šmarno goro</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>smartnoB</t>
-        </is>
-      </c>
-      <c r="D25" t="n">
-        <v>6</v>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>Zakaj je Replja rekla Puhanki, da ni ravno ena najpametnejših? / Why did Replja say that Puhanka is "Not one of the smartest ones"?</t>
-        </is>
-      </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>Book Club Two</t>
-        </is>
-      </c>
-      <c r="G25" t="n">
-        <v>824</v>
-      </c>
-      <c r="H25" t="inlineStr">
-        <is>
-          <t>smartnoB20</t>
-        </is>
-      </c>
-      <c r="I25" t="inlineStr">
-        <is>
-          <t>MMMMMMMMMMMMMMMMM NE VEM</t>
-        </is>
-      </c>
-      <c r="J25" t="inlineStr">
-        <is>
-          <t>MMMMMMMMMMMMMMM I DON'T KNOW</t>
-        </is>
-      </c>
-      <c r="K25" s="2" t="n">
-        <v>43581.14689814814</v>
-      </c>
-      <c r="L25" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="M25" t="n">
-        <v>14</v>
-      </c>
-      <c r="N25" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="O25" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="P25" t="inlineStr">
-        <is>
-          <t>DA</t>
-        </is>
-      </c>
-      <c r="Q25" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="1" t="n">
-        <v>3506</v>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>OŠ Šmartno pod Šmarno goro</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>smartnoB</t>
-        </is>
-      </c>
-      <c r="D26" t="n">
-        <v>8</v>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>Kaj pa bi lahko v tvojem kraju naredili, da bi bilo manj takšnih otrok, ki nimajo kaj obleči? / What could your community do to make sure there were less kids with nothing to wear?</t>
-        </is>
-      </c>
-      <c r="F26" t="inlineStr">
-        <is>
-          <t>Book Club One</t>
-        </is>
-      </c>
-      <c r="G26" t="n">
-        <v>823</v>
-      </c>
-      <c r="H26" t="inlineStr">
-        <is>
-          <t>smartnoB19</t>
-        </is>
-      </c>
-      <c r="I26" t="inlineStr">
-        <is>
-          <t>Ja jaz sem punca</t>
-        </is>
-      </c>
-      <c r="J26" t="inlineStr">
-        <is>
-          <t>Yes I am a girl</t>
-        </is>
-      </c>
-      <c r="K26" s="2" t="n">
-        <v>43581.12827546296</v>
-      </c>
-      <c r="L26" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="M26" t="n">
-        <v>6</v>
-      </c>
-      <c r="N26" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="O26" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="P26" t="inlineStr">
-        <is>
-          <t>CO</t>
-        </is>
-      </c>
-      <c r="Q26" t="inlineStr">
         <is>
           <t>C</t>
         </is>

</xml_diff>

<commit_message>
fixes, add results to README
</commit_message>
<xml_diff>
--- a/results/fn.xlsx
+++ b/results/fn.xlsx
@@ -362,7 +362,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q33"/>
+  <dimension ref="A1:Q24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -531,7 +531,7 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>3213</v>
+        <v>3223</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -548,7 +548,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Kako bi Kekec na drugačen način prišel do zdravila? / In what other way could Kekec get the medicine?</t>
+          <t>Kako pa bi se ti počutil/-a, če bi moral/-a zapustiti svojo družino? Zakaj? / How would you feel if you had to leave your family? Why?</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -557,25 +557,25 @@
         </is>
       </c>
       <c r="G3" t="n">
-        <v>718</v>
+        <v>722</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>filipkrstic</t>
+          <t>mariapavela</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>ne ker noce</t>
+          <t>jaz tudi ne</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t xml:space="preserve">No because she doesn't want to </t>
+          <t>Me neither</t>
         </is>
       </c>
       <c r="K3" s="2" t="n">
-        <v>43536.26443287037</v>
+        <v>43536.23633101852</v>
       </c>
       <c r="L3" t="inlineStr">
         <is>
@@ -583,7 +583,7 @@
         </is>
       </c>
       <c r="M3" t="n">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="N3" t="inlineStr">
         <is>
@@ -608,7 +608,7 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>3214</v>
+        <v>3231</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -625,7 +625,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Kako bi Kekec na drugačen način prišel do zdravila? / In what other way could Kekec get the medicine?</t>
+          <t>Mojca je bila prepričana, da je z njo ženska iz vasi. Ali misliš, da bi drugače vseeno odšla s Pehto? Zakaj? / Mojca was sure, that the woman she met was someone from the village. Do you think she would still leave with Pehta if she thought otherwise? Why?</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -634,25 +634,25 @@
         </is>
       </c>
       <c r="G4" t="n">
-        <v>722</v>
+        <v>718</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>mariapavela</t>
+          <t>filipkrstic</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>ja ampak zakaj noče</t>
+          <t>aja</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Yes but why doesn't she want to?</t>
+          <t>Oh</t>
         </is>
       </c>
       <c r="K4" s="2" t="n">
-        <v>43536.26611111111</v>
+        <v>43536.24097222222</v>
       </c>
       <c r="L4" t="inlineStr">
         <is>
@@ -660,7 +660,7 @@
         </is>
       </c>
       <c r="M4" t="n">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="N4" t="inlineStr">
         <is>
@@ -669,12 +669,12 @@
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>Q</t>
+          <t>A</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>DQ</t>
+          <t>DAA</t>
         </is>
       </c>
       <c r="Q4" t="inlineStr">
@@ -685,7 +685,7 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>3231</v>
+        <v>3233</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -729,7 +729,7 @@
         </is>
       </c>
       <c r="K5" s="2" t="n">
-        <v>43536.24097222222</v>
+        <v>43536.24106481481</v>
       </c>
       <c r="L5" t="inlineStr">
         <is>
@@ -762,7 +762,7 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>3233</v>
+        <v>3239</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -788,25 +788,25 @@
         </is>
       </c>
       <c r="G6" t="n">
-        <v>718</v>
+        <v>720</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>filipkrstic</t>
+          <t>tijanamiljanovic</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>aja</t>
+          <t>jp</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>Oh</t>
+          <t>Yep</t>
         </is>
       </c>
       <c r="K6" s="2" t="n">
-        <v>43536.24106481481</v>
+        <v>43536.24672453704</v>
       </c>
       <c r="L6" t="inlineStr">
         <is>
@@ -814,7 +814,7 @@
         </is>
       </c>
       <c r="M6" t="n">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="N6" t="inlineStr">
         <is>
@@ -828,7 +828,7 @@
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>DAA</t>
+          <t>DA</t>
         </is>
       </c>
       <c r="Q6" t="inlineStr">
@@ -839,7 +839,7 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>3239</v>
+        <v>3241</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -874,16 +874,16 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>jp</t>
+          <t>jaz pa ne zakaj</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>Yep</t>
+          <t>I wouldn't want to be him. Why (would you want to be him)?</t>
         </is>
       </c>
       <c r="K7" s="2" t="n">
-        <v>43536.24672453704</v>
+        <v>43536.25361111111</v>
       </c>
       <c r="L7" t="inlineStr">
         <is>
@@ -891,7 +891,7 @@
         </is>
       </c>
       <c r="M7" t="n">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="N7" t="inlineStr">
         <is>
@@ -900,12 +900,12 @@
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>Q</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>DA</t>
+          <t>DQ</t>
         </is>
       </c>
       <c r="Q7" t="inlineStr">
@@ -916,7 +916,7 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>3241</v>
+        <v>3242</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -942,25 +942,25 @@
         </is>
       </c>
       <c r="G8" t="n">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>tijanamiljanovic</t>
+          <t>filipkrstic</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>jaz pa ne zakaj</t>
+          <t>hecam se mojca</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>I wouldn't want to be him. Why (would you want to be him)?</t>
+          <t>I'm kidding, (I'd want to be) Mojca</t>
         </is>
       </c>
       <c r="K8" s="2" t="n">
-        <v>43536.25361111111</v>
+        <v>43536.25422453704</v>
       </c>
       <c r="L8" t="inlineStr">
         <is>
@@ -968,7 +968,7 @@
         </is>
       </c>
       <c r="M8" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N8" t="inlineStr">
         <is>
@@ -977,12 +977,12 @@
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>Q</t>
+          <t>A</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t>DQ</t>
+          <t>DAA</t>
         </is>
       </c>
       <c r="Q8" t="inlineStr">
@@ -993,7 +993,7 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>3242</v>
+        <v>3245</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -1019,25 +1019,25 @@
         </is>
       </c>
       <c r="G9" t="n">
-        <v>718</v>
+        <v>720</v>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>filipkrstic</t>
+          <t>tijanamiljanovic</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>hecam se mojca</t>
+          <t>oprosti mojca</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>I'm kidding, (I'd want to be) Mojca</t>
+          <t>I'm sorry Mojca</t>
         </is>
       </c>
       <c r="K9" s="2" t="n">
-        <v>43536.25422453704</v>
+        <v>43536.25638888889</v>
       </c>
       <c r="L9" t="inlineStr">
         <is>
@@ -1045,7 +1045,7 @@
         </is>
       </c>
       <c r="M9" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="N9" t="inlineStr">
         <is>
@@ -1070,7 +1070,7 @@
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>3245</v>
+        <v>3253</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -1087,34 +1087,34 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Mojca je bila prepričana, da je z njo ženska iz vasi. Ali misliš, da bi drugače vseeno odšla s Pehto? Zakaj? / Mojca was sure, that the woman she met was someone from the village. Do you think she would still leave with Pehta if she thought otherwise? Why?</t>
+          <t>Kako pa bi se ti počutil/-a, če bi moral/-a zapustiti svojo družino? Zakaj? / How would you feel if you had to leave your family? Why?</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Knjižni Klub 7</t>
+          <t>Knjižni Klub 8</t>
         </is>
       </c>
       <c r="G10" t="n">
-        <v>720</v>
+        <v>726</v>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>tijanamiljanovic</t>
+          <t>timskander</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>oprosti mojca</t>
+          <t>prestrašeno</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>I'm sorry Mojca</t>
+          <t>scared</t>
         </is>
       </c>
       <c r="K10" s="2" t="n">
-        <v>43536.25638888889</v>
+        <v>43536.23680555556</v>
       </c>
       <c r="L10" t="inlineStr">
         <is>
@@ -1122,7 +1122,7 @@
         </is>
       </c>
       <c r="M10" t="n">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="N10" t="inlineStr">
         <is>
@@ -1136,7 +1136,7 @@
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>DAA</t>
+          <t>DA</t>
         </is>
       </c>
       <c r="Q10" t="inlineStr">
@@ -1147,7 +1147,7 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>3253</v>
+        <v>3258</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -1164,7 +1164,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Kako pa bi se ti počutil/-a, če bi moral/-a zapustiti svojo družino? Zakaj? / How would you feel if you had to leave your family? Why?</t>
+          <t>Mojca je bila prepričana, da je z njo ženska iz vasi. Ali misliš, da bi drugače vseeno odšla s Pehto? Zakaj? / Mojca was sure, that the woman she met was someone from the village. Do you think she would still leave with Pehta if she thought otherwise? Why?</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1173,21 +1173,21 @@
         </is>
       </c>
       <c r="G11" t="n">
-        <v>726</v>
+        <v>723</v>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>timskander</t>
+          <t>ajdapelicon</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>prestrašeno</t>
+          <t>po moje ne</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>scared</t>
+          <t xml:space="preserve">I don't think so. </t>
         </is>
       </c>
       <c r="K11" s="2" t="n">
@@ -1199,7 +1199,7 @@
         </is>
       </c>
       <c r="M11" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="N11" t="inlineStr">
         <is>
@@ -1224,7 +1224,7 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>3257</v>
+        <v>3263</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -1259,20 +1259,20 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>Ne nebi odšla s Pehto</t>
+          <t>itak</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t xml:space="preserve">No she wouldn't have left with Pehta. </t>
+          <t xml:space="preserve">Of course. </t>
         </is>
       </c>
       <c r="K12" s="2" t="n">
-        <v>43536.18680555555</v>
+        <v>43536.26666666667</v>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="M12" t="n">
@@ -1301,51 +1301,51 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>3258</v>
+        <v>3276</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>OŠ Koseze</t>
+          <t>OŠ Šmartno pod Šmarno goro</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Koseze</t>
+          <t>Smartno</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Mojca je bila prepričana, da je z njo ženska iz vasi. Ali misliš, da bi drugače vseeno odšla s Pehto? Zakaj? / Mojca was sure, that the woman she met was someone from the village. Do you think she would still leave with Pehta if she thought otherwise? Why?</t>
+          <t>Kako bi Kekec na drugačen način prišel do zdravila? / In what other way could Kekec get the medicine?</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Knjižni Klub 8</t>
+          <t>Book Club One</t>
         </is>
       </c>
       <c r="G13" t="n">
-        <v>723</v>
+        <v>793</v>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>ajdapelicon</t>
+          <t>smartno20</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>po moje ne</t>
+          <t>ja da bimu pehta skuhala</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t xml:space="preserve">I don't think so. </t>
+          <t>That Pehta would cook it for him</t>
         </is>
       </c>
       <c r="K13" s="2" t="n">
-        <v>43536.23680555556</v>
+        <v>43574.16180555556</v>
       </c>
       <c r="L13" t="inlineStr">
         <is>
@@ -1353,7 +1353,7 @@
         </is>
       </c>
       <c r="M13" t="n">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="N13" t="inlineStr">
         <is>
@@ -1378,51 +1378,51 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>3263</v>
+        <v>3312</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>OŠ Koseze</t>
+          <t>OŠ Šmartno pod Šmarno goro</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Koseze</t>
+          <t>Smartno</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Mojca je bila prepričana, da je z njo ženska iz vasi. Ali misliš, da bi drugače vseeno odšla s Pehto? Zakaj? / Mojca was sure, that the woman she met was someone from the village. Do you think she would still leave with Pehta if she thought otherwise? Why?</t>
+          <t>Zakaj je Replja rekla Puhanki, da ni ravno ena najpametnejših? / Why did Replja say that Puhanka is "Not one of the smartest ones"?</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Knjižni Klub 8</t>
+          <t>Book Club Three</t>
         </is>
       </c>
       <c r="G14" t="n">
-        <v>676</v>
+        <v>781</v>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>karin japelj K</t>
+          <t>smartno8</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>itak</t>
+          <t>enako</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t xml:space="preserve">Of course. </t>
+          <t>Same</t>
         </is>
       </c>
       <c r="K14" s="2" t="n">
-        <v>43536.26666666667</v>
+        <v>43574.14583333334</v>
       </c>
       <c r="L14" t="inlineStr">
         <is>
@@ -1430,7 +1430,7 @@
         </is>
       </c>
       <c r="M14" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="N14" t="inlineStr">
         <is>
@@ -1439,12 +1439,12 @@
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>S</t>
         </is>
       </c>
       <c r="P14" t="inlineStr">
         <is>
-          <t>DA</t>
+          <t>DAA</t>
         </is>
       </c>
       <c r="Q14" t="inlineStr">
@@ -1455,7 +1455,7 @@
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>3273</v>
+        <v>3329</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
@@ -1468,38 +1468,38 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Kako bi Kekec na drugačen način prišel do zdravila? / In what other way could Kekec get the medicine?</t>
+          <t>Zakaj je Replja rekla Puhanki, da ni ravno ena najpametnejših? / Why did Replja say that Puhanka is "Not one of the smartest ones"?</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Book Club One</t>
+          <t>Book Club Four</t>
         </is>
       </c>
       <c r="G15" t="n">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>smartno12</t>
+          <t>smartno11</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>maš ti kakšno idejo?</t>
+          <t>ja verjetno res</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>Do you have any ideas?</t>
+          <t>Yes you are probably right</t>
         </is>
       </c>
       <c r="K15" s="2" t="n">
-        <v>43574.16041666667</v>
+        <v>43574.15416666667</v>
       </c>
       <c r="L15" t="inlineStr">
         <is>
@@ -1507,7 +1507,7 @@
         </is>
       </c>
       <c r="M15" t="n">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="N15" t="inlineStr">
         <is>
@@ -1516,12 +1516,12 @@
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>Q</t>
+          <t>S</t>
         </is>
       </c>
       <c r="P15" t="inlineStr">
         <is>
-          <t>DA</t>
+          <t>DAA</t>
         </is>
       </c>
       <c r="Q15" t="inlineStr">
@@ -1532,7 +1532,7 @@
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>3275</v>
+        <v>3330</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
@@ -1545,38 +1545,38 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Kako bi Kekec na drugačen način prišel do zdravila? / In what other way could Kekec get the medicine?</t>
+          <t>Zakaj je Replja rekla Puhanki, da ni ravno ena najpametnejših? / Why did Replja say that Puhanka is "Not one of the smartest ones"?</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Book Club One</t>
+          <t>Book Club Four</t>
         </is>
       </c>
       <c r="G16" t="n">
-        <v>796</v>
+        <v>784</v>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>smartno23</t>
+          <t>smartno11</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>Z čem že</t>
+          <t>ubistvu nevem ravno</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>With what</t>
+          <t>Actually I don't really know</t>
         </is>
       </c>
       <c r="K16" s="2" t="n">
-        <v>43574.16111111111</v>
+        <v>43574.15694444445</v>
       </c>
       <c r="L16" t="inlineStr">
         <is>
@@ -1584,7 +1584,7 @@
         </is>
       </c>
       <c r="M16" t="n">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="N16" t="inlineStr">
         <is>
@@ -1593,23 +1593,23 @@
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>Q</t>
+          <t>S</t>
         </is>
       </c>
       <c r="P16" t="inlineStr">
         <is>
-          <t>CO</t>
+          <t>DAA</t>
         </is>
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>D</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>3278</v>
+        <v>3334</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
@@ -1622,47 +1622,47 @@
         </is>
       </c>
       <c r="D17" t="n">
+        <v>7</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Kako bi lahko Cefizelj pobegnil policistu še na drugačen način? / In what other way could Cefizelj get away from the policeman?</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Book Club One</t>
+        </is>
+      </c>
+      <c r="G17" t="n">
+        <v>793</v>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>smartno20</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>nevem</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>I don't know</t>
+        </is>
+      </c>
+      <c r="K17" s="2" t="n">
+        <v>43574.13263888889</v>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="M17" t="n">
         <v>5</v>
       </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>Kako bi Kekec na drugačen način prišel do zdravila? / In what other way could Kekec get the medicine?</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>Book Club One</t>
-        </is>
-      </c>
-      <c r="G17" t="n">
-        <v>785</v>
-      </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>smartno12</t>
-        </is>
-      </c>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>joj nevem  no ja ubistvu vem</t>
-        </is>
-      </c>
-      <c r="J17" t="inlineStr">
-        <is>
-          <t>Well I don't know well actually I do</t>
-        </is>
-      </c>
-      <c r="K17" s="2" t="n">
-        <v>43574.16180555556</v>
-      </c>
-      <c r="L17" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="M17" t="n">
-        <v>17</v>
-      </c>
       <c r="N17" t="inlineStr">
         <is>
           <t>Yes</t>
@@ -1670,23 +1670,23 @@
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>A</t>
         </is>
       </c>
       <c r="P17" t="inlineStr">
         <is>
-          <t>CO</t>
+          <t>DA</t>
         </is>
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>D</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>3306</v>
+        <v>3335</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
@@ -1699,38 +1699,38 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Zakaj je Replja rekla Puhanki, da ni ravno ena najpametnejših? / Why did Replja say that Puhanka is "Not one of the smartest ones"?</t>
+          <t>Kako bi lahko Cefizelj pobegnil policistu še na drugačen način? / In what other way could Cefizelj get away from the policeman?</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Book Club Two</t>
+          <t>Book Club One</t>
         </is>
       </c>
       <c r="G18" t="n">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>smartno10</t>
+          <t>smartno12</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>mama Puhlanka je bila tako:muahahahaha</t>
+          <t>mmmm NEVEMM</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>mother Puhljanka was like: muahahahah</t>
+          <t>mmmmm I DON'T KNOW</t>
         </is>
       </c>
       <c r="K18" s="2" t="n">
-        <v>43574.14722222222</v>
+        <v>43574.13611111111</v>
       </c>
       <c r="L18" t="inlineStr">
         <is>
@@ -1738,7 +1738,7 @@
         </is>
       </c>
       <c r="M18" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="N18" t="inlineStr">
         <is>
@@ -1763,7 +1763,7 @@
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>3307</v>
+        <v>3343</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
@@ -1776,11 +1776,11 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Zakaj je Replja rekla Puhanki, da ni ravno ena najpametnejših? / Why did Replja say that Puhanka is "Not one of the smartest ones"?</t>
+          <t>Kako bi lahko Cefizelj pobegnil policistu še na drugačen način? / In what other way could Cefizelj get away from the policeman?</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1798,16 +1798,16 @@
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>mama se je razjezila</t>
+          <t>kam</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t xml:space="preserve">mom was angry </t>
+          <t>Where</t>
         </is>
       </c>
       <c r="K19" s="2" t="n">
-        <v>43574.15902777778</v>
+        <v>43574.14652777778</v>
       </c>
       <c r="L19" t="inlineStr">
         <is>
@@ -1815,7 +1815,7 @@
         </is>
       </c>
       <c r="M19" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="N19" t="inlineStr">
         <is>
@@ -1824,12 +1824,12 @@
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>Q</t>
         </is>
       </c>
       <c r="P19" t="inlineStr">
         <is>
-          <t>DA</t>
+          <t>DQ</t>
         </is>
       </c>
       <c r="Q19" t="inlineStr">
@@ -1840,7 +1840,7 @@
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>3328</v>
+        <v>3376</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
@@ -1853,47 +1853,47 @@
         </is>
       </c>
       <c r="D20" t="n">
+        <v>8</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Kaj pa bi lahko v tvojem kraju naredili, da bi bilo manj takšnih otrok, ki nimajo kaj obleči? / What could your community do to make sure there were less kids with nothing to wear?</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Book Club One</t>
+        </is>
+      </c>
+      <c r="G20" t="n">
+        <v>793</v>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>smartno20</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>jaz isto</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>Me too</t>
+        </is>
+      </c>
+      <c r="K20" s="2" t="n">
+        <v>43574.12361111111</v>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="M20" t="n">
         <v>6</v>
       </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>Zakaj je Replja rekla Puhanki, da ni ravno ena najpametnejših? / Why did Replja say that Puhanka is "Not one of the smartest ones"?</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>Book Club Four</t>
-        </is>
-      </c>
-      <c r="G20" t="n">
-        <v>792</v>
-      </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>smartno19</t>
-        </is>
-      </c>
-      <c r="I20" t="inlineStr">
-        <is>
-          <t>no saj tako se mi zdi</t>
-        </is>
-      </c>
-      <c r="J20" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Well at least I think so </t>
-        </is>
-      </c>
-      <c r="K20" s="2" t="n">
-        <v>43574.14444444444</v>
-      </c>
-      <c r="L20" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="M20" t="n">
-        <v>10</v>
-      </c>
       <c r="N20" t="inlineStr">
         <is>
           <t>Yes</t>
@@ -1901,7 +1901,7 @@
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>A</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
@@ -1917,7 +1917,7 @@
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>3329</v>
+        <v>3408</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
@@ -1930,47 +1930,47 @@
         </is>
       </c>
       <c r="D21" t="n">
+        <v>8</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Kaj pa bi lahko v tvojem kraju naredili, da bi bilo manj takšnih otrok, ki nimajo kaj obleči? / What could your community do to make sure there were less kids with nothing to wear?</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Book Club Three</t>
+        </is>
+      </c>
+      <c r="G21" t="n">
+        <v>782</v>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>smartno9</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>RAZDAL</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>GIVE AWAY</t>
+        </is>
+      </c>
+      <c r="K21" s="2" t="n">
+        <v>43574.12916666667</v>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="M21" t="n">
         <v>6</v>
       </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>Zakaj je Replja rekla Puhanki, da ni ravno ena najpametnejših? / Why did Replja say that Puhanka is "Not one of the smartest ones"?</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>Book Club Four</t>
-        </is>
-      </c>
-      <c r="G21" t="n">
-        <v>784</v>
-      </c>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>smartno11</t>
-        </is>
-      </c>
-      <c r="I21" t="inlineStr">
-        <is>
-          <t>ja verjetno res</t>
-        </is>
-      </c>
-      <c r="J21" t="inlineStr">
-        <is>
-          <t>Yes you are probably right</t>
-        </is>
-      </c>
-      <c r="K21" s="2" t="n">
-        <v>43574.15416666667</v>
-      </c>
-      <c r="L21" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="M21" t="n">
-        <v>11</v>
-      </c>
       <c r="N21" t="inlineStr">
         <is>
           <t>Yes</t>
@@ -1978,12 +1978,12 @@
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>A</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
         <is>
-          <t>DAA</t>
+          <t>DA</t>
         </is>
       </c>
       <c r="Q21" t="inlineStr">
@@ -1994,7 +1994,7 @@
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>3330</v>
+        <v>3453</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
@@ -2003,7 +2003,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Smartno</t>
+          <t>smartnoB</t>
         </is>
       </c>
       <c r="D22" t="n">
@@ -2016,29 +2016,29 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Book Club Four</t>
+          <t>Book Club One</t>
         </is>
       </c>
       <c r="G22" t="n">
-        <v>784</v>
+        <v>816</v>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>smartno11</t>
+          <t>smartnoB12</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>ubistvu nevem ravno</t>
+          <t>Nevem</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>Actually I don't really know</t>
+          <t>I don't know</t>
         </is>
       </c>
       <c r="K22" s="2" t="n">
-        <v>43574.15694444445</v>
+        <v>43581.15891203703</v>
       </c>
       <c r="L22" t="inlineStr">
         <is>
@@ -2046,7 +2046,7 @@
         </is>
       </c>
       <c r="M22" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="N22" t="inlineStr">
         <is>
@@ -2055,12 +2055,12 @@
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>A</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
         <is>
-          <t>DAA</t>
+          <t>DA</t>
         </is>
       </c>
       <c r="Q22" t="inlineStr">
@@ -2071,7 +2071,7 @@
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>3331</v>
+        <v>3460</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
@@ -2080,7 +2080,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Smartno</t>
+          <t>smartnoB</t>
         </is>
       </c>
       <c r="D23" t="n">
@@ -2093,29 +2093,29 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Book Club Four</t>
+          <t>Book Club Two</t>
         </is>
       </c>
       <c r="G23" t="n">
-        <v>786</v>
+        <v>824</v>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>smartno13</t>
+          <t>smartnoB20</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>ker je skakanje najboljše</t>
+          <t>MMMMMMMMMMMMMMMMM NE VEM</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>Because jumping is the best</t>
+          <t>MMMMMMMMMMMMMMM I DON'T KNOW</t>
         </is>
       </c>
       <c r="K23" s="2" t="n">
-        <v>43574.16111111111</v>
+        <v>43581.14689814814</v>
       </c>
       <c r="L23" t="inlineStr">
         <is>
@@ -2123,7 +2123,7 @@
         </is>
       </c>
       <c r="M23" t="n">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="N23" t="inlineStr">
         <is>
@@ -2148,7 +2148,7 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>3335</v>
+        <v>3506</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
@@ -2157,15 +2157,15 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Smartno</t>
+          <t>smartnoB</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Kako bi lahko Cefizelj pobegnil policistu še na drugačen način? / In what other way could Cefizelj get away from the policeman?</t>
+          <t>Kaj pa bi lahko v tvojem kraju naredili, da bi bilo manj takšnih otrok, ki nimajo kaj obleči? / What could your community do to make sure there were less kids with nothing to wear?</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2174,25 +2174,25 @@
         </is>
       </c>
       <c r="G24" t="n">
-        <v>785</v>
+        <v>823</v>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>smartno12</t>
+          <t>smartnoB19</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>mmmm NEVEMM</t>
+          <t>Ja jaz sem punca</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>mmmmm I DON'T KNOW</t>
+          <t>Yes I am a girl</t>
         </is>
       </c>
       <c r="K24" s="2" t="n">
-        <v>43574.13611111111</v>
+        <v>43581.12827546296</v>
       </c>
       <c r="L24" t="inlineStr">
         <is>
@@ -2200,7 +2200,7 @@
         </is>
       </c>
       <c r="M24" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="N24" t="inlineStr">
         <is>
@@ -2209,708 +2209,15 @@
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>A</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
         <is>
-          <t>DA</t>
+          <t>CO</t>
         </is>
       </c>
       <c r="Q24" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="1" t="n">
-        <v>3343</v>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>OŠ Šmartno pod Šmarno goro</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>Smartno</t>
-        </is>
-      </c>
-      <c r="D25" t="n">
-        <v>7</v>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>Kako bi lahko Cefizelj pobegnil policistu še na drugačen način? / In what other way could Cefizelj get away from the policeman?</t>
-        </is>
-      </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>Book Club Two</t>
-        </is>
-      </c>
-      <c r="G25" t="n">
-        <v>794</v>
-      </c>
-      <c r="H25" t="inlineStr">
-        <is>
-          <t>smartno21</t>
-        </is>
-      </c>
-      <c r="I25" t="inlineStr">
-        <is>
-          <t>kam</t>
-        </is>
-      </c>
-      <c r="J25" t="inlineStr">
-        <is>
-          <t>Where</t>
-        </is>
-      </c>
-      <c r="K25" s="2" t="n">
-        <v>43574.14652777778</v>
-      </c>
-      <c r="L25" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="M25" t="n">
-        <v>5</v>
-      </c>
-      <c r="N25" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="O25" t="inlineStr">
-        <is>
-          <t>Q</t>
-        </is>
-      </c>
-      <c r="P25" t="inlineStr">
-        <is>
-          <t>DQ</t>
-        </is>
-      </c>
-      <c r="Q25" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="1" t="n">
-        <v>3375</v>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>OŠ Šmartno pod Šmarno goro</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>Smartno</t>
-        </is>
-      </c>
-      <c r="D26" t="n">
-        <v>8</v>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>Kaj pa bi lahko v tvojem kraju naredili, da bi bilo manj takšnih otrok, ki nimajo kaj obleči? / What could your community do to make sure there were less kids with nothing to wear?</t>
-        </is>
-      </c>
-      <c r="F26" t="inlineStr">
-        <is>
-          <t>Book Club One</t>
-        </is>
-      </c>
-      <c r="G26" t="n">
-        <v>796</v>
-      </c>
-      <c r="H26" t="inlineStr">
-        <is>
-          <t>smartno23</t>
-        </is>
-      </c>
-      <c r="I26" t="inlineStr">
-        <is>
-          <t>jaz bi jim posodil dnar</t>
-        </is>
-      </c>
-      <c r="J26" t="inlineStr">
-        <is>
-          <t>I would lend them money</t>
-        </is>
-      </c>
-      <c r="K26" s="2" t="n">
-        <v>43574.12222222222</v>
-      </c>
-      <c r="L26" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="M26" t="n">
-        <v>6</v>
-      </c>
-      <c r="N26" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="O26" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="P26" t="inlineStr">
-        <is>
-          <t>DA</t>
-        </is>
-      </c>
-      <c r="Q26" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="1" t="n">
-        <v>3376</v>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>OŠ Šmartno pod Šmarno goro</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>Smartno</t>
-        </is>
-      </c>
-      <c r="D27" t="n">
-        <v>8</v>
-      </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>Kaj pa bi lahko v tvojem kraju naredili, da bi bilo manj takšnih otrok, ki nimajo kaj obleči? / What could your community do to make sure there were less kids with nothing to wear?</t>
-        </is>
-      </c>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>Book Club One</t>
-        </is>
-      </c>
-      <c r="G27" t="n">
-        <v>793</v>
-      </c>
-      <c r="H27" t="inlineStr">
-        <is>
-          <t>smartno20</t>
-        </is>
-      </c>
-      <c r="I27" t="inlineStr">
-        <is>
-          <t>jaz isto</t>
-        </is>
-      </c>
-      <c r="J27" t="inlineStr">
-        <is>
-          <t>Me too</t>
-        </is>
-      </c>
-      <c r="K27" s="2" t="n">
-        <v>43574.12361111111</v>
-      </c>
-      <c r="L27" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="M27" t="n">
-        <v>6</v>
-      </c>
-      <c r="N27" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="O27" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="P27" t="inlineStr">
-        <is>
-          <t>DAA</t>
-        </is>
-      </c>
-      <c r="Q27" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="1" t="n">
-        <v>3377</v>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>OŠ Šmartno pod Šmarno goro</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>Smartno</t>
-        </is>
-      </c>
-      <c r="D28" t="n">
-        <v>8</v>
-      </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>Kaj pa bi lahko v tvojem kraju naredili, da bi bilo manj takšnih otrok, ki nimajo kaj obleči? / What could your community do to make sure there were less kids with nothing to wear?</t>
-        </is>
-      </c>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t>Book Club One</t>
-        </is>
-      </c>
-      <c r="G28" t="n">
-        <v>796</v>
-      </c>
-      <c r="H28" t="inlineStr">
-        <is>
-          <t>smartno23</t>
-        </is>
-      </c>
-      <c r="I28" t="inlineStr">
-        <is>
-          <t>zakaj že</t>
-        </is>
-      </c>
-      <c r="J28" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Why would you </t>
-        </is>
-      </c>
-      <c r="K28" s="2" t="n">
-        <v>43574.125</v>
-      </c>
-      <c r="L28" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="M28" t="n">
-        <v>7</v>
-      </c>
-      <c r="N28" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="O28" t="inlineStr">
-        <is>
-          <t>Q</t>
-        </is>
-      </c>
-      <c r="P28" t="inlineStr">
-        <is>
-          <t>DQ</t>
-        </is>
-      </c>
-      <c r="Q28" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" s="1" t="n">
-        <v>3408</v>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>OŠ Šmartno pod Šmarno goro</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>Smartno</t>
-        </is>
-      </c>
-      <c r="D29" t="n">
-        <v>8</v>
-      </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>Kaj pa bi lahko v tvojem kraju naredili, da bi bilo manj takšnih otrok, ki nimajo kaj obleči? / What could your community do to make sure there were less kids with nothing to wear?</t>
-        </is>
-      </c>
-      <c r="F29" t="inlineStr">
-        <is>
-          <t>Book Club Three</t>
-        </is>
-      </c>
-      <c r="G29" t="n">
-        <v>782</v>
-      </c>
-      <c r="H29" t="inlineStr">
-        <is>
-          <t>smartno9</t>
-        </is>
-      </c>
-      <c r="I29" t="inlineStr">
-        <is>
-          <t>RAZDAL</t>
-        </is>
-      </c>
-      <c r="J29" t="inlineStr">
-        <is>
-          <t>GIVE AWAY</t>
-        </is>
-      </c>
-      <c r="K29" s="2" t="n">
-        <v>43574.12916666667</v>
-      </c>
-      <c r="L29" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="M29" t="n">
-        <v>6</v>
-      </c>
-      <c r="N29" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="O29" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="P29" t="inlineStr">
-        <is>
-          <t>DA</t>
-        </is>
-      </c>
-      <c r="Q29" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="1" t="n">
-        <v>3432</v>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>OŠ Šmartno pod Šmarno goro</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>Smartno</t>
-        </is>
-      </c>
-      <c r="D30" t="n">
-        <v>8</v>
-      </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>Kaj pa bi lahko v tvojem kraju naredili, da bi bilo manj takšnih otrok, ki nimajo kaj obleči? / What could your community do to make sure there were less kids with nothing to wear?</t>
-        </is>
-      </c>
-      <c r="F30" t="inlineStr">
-        <is>
-          <t>Book Club Four</t>
-        </is>
-      </c>
-      <c r="G30" t="n">
-        <v>779</v>
-      </c>
-      <c r="H30" t="inlineStr">
-        <is>
-          <t>smartno6</t>
-        </is>
-      </c>
-      <c r="I30" t="inlineStr">
-        <is>
-          <t>kopili  bi jim srajco                            odpišite   mi</t>
-        </is>
-      </c>
-      <c r="J30" t="inlineStr">
-        <is>
-          <t>I would buy them a shirt          write back to me</t>
-        </is>
-      </c>
-      <c r="K30" s="2" t="n">
-        <v>43574.12708333333</v>
-      </c>
-      <c r="L30" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="M30" t="n">
-        <v>6</v>
-      </c>
-      <c r="N30" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="O30" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="P30" t="inlineStr">
-        <is>
-          <t>DA</t>
-        </is>
-      </c>
-      <c r="Q30" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="1" t="n">
-        <v>3453</v>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>OŠ Šmartno pod Šmarno goro</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>smartnoB</t>
-        </is>
-      </c>
-      <c r="D31" t="n">
-        <v>6</v>
-      </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>Zakaj je Replja rekla Puhanki, da ni ravno ena najpametnejših? / Why did Replja say that Puhanka is "Not one of the smartest ones"?</t>
-        </is>
-      </c>
-      <c r="F31" t="inlineStr">
-        <is>
-          <t>Book Club One</t>
-        </is>
-      </c>
-      <c r="G31" t="n">
-        <v>816</v>
-      </c>
-      <c r="H31" t="inlineStr">
-        <is>
-          <t>smartnoB12</t>
-        </is>
-      </c>
-      <c r="I31" t="inlineStr">
-        <is>
-          <t>Nevem</t>
-        </is>
-      </c>
-      <c r="J31" t="inlineStr">
-        <is>
-          <t>I don't know</t>
-        </is>
-      </c>
-      <c r="K31" s="2" t="n">
-        <v>43581.15891203703</v>
-      </c>
-      <c r="L31" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="M31" t="n">
-        <v>10</v>
-      </c>
-      <c r="N31" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="O31" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="P31" t="inlineStr">
-        <is>
-          <t>DA</t>
-        </is>
-      </c>
-      <c r="Q31" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="1" t="n">
-        <v>3460</v>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>OŠ Šmartno pod Šmarno goro</t>
-        </is>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>smartnoB</t>
-        </is>
-      </c>
-      <c r="D32" t="n">
-        <v>6</v>
-      </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>Zakaj je Replja rekla Puhanki, da ni ravno ena najpametnejših? / Why did Replja say that Puhanka is "Not one of the smartest ones"?</t>
-        </is>
-      </c>
-      <c r="F32" t="inlineStr">
-        <is>
-          <t>Book Club Two</t>
-        </is>
-      </c>
-      <c r="G32" t="n">
-        <v>824</v>
-      </c>
-      <c r="H32" t="inlineStr">
-        <is>
-          <t>smartnoB20</t>
-        </is>
-      </c>
-      <c r="I32" t="inlineStr">
-        <is>
-          <t>MMMMMMMMMMMMMMMMM NE VEM</t>
-        </is>
-      </c>
-      <c r="J32" t="inlineStr">
-        <is>
-          <t>MMMMMMMMMMMMMMM I DON'T KNOW</t>
-        </is>
-      </c>
-      <c r="K32" s="2" t="n">
-        <v>43581.14689814814</v>
-      </c>
-      <c r="L32" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="M32" t="n">
-        <v>14</v>
-      </c>
-      <c r="N32" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="O32" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="P32" t="inlineStr">
-        <is>
-          <t>DA</t>
-        </is>
-      </c>
-      <c r="Q32" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="1" t="n">
-        <v>3506</v>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>OŠ Šmartno pod Šmarno goro</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>smartnoB</t>
-        </is>
-      </c>
-      <c r="D33" t="n">
-        <v>8</v>
-      </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>Kaj pa bi lahko v tvojem kraju naredili, da bi bilo manj takšnih otrok, ki nimajo kaj obleči? / What could your community do to make sure there were less kids with nothing to wear?</t>
-        </is>
-      </c>
-      <c r="F33" t="inlineStr">
-        <is>
-          <t>Book Club One</t>
-        </is>
-      </c>
-      <c r="G33" t="n">
-        <v>823</v>
-      </c>
-      <c r="H33" t="inlineStr">
-        <is>
-          <t>smartnoB19</t>
-        </is>
-      </c>
-      <c r="I33" t="inlineStr">
-        <is>
-          <t>Ja jaz sem punca</t>
-        </is>
-      </c>
-      <c r="J33" t="inlineStr">
-        <is>
-          <t>Yes I am a girl</t>
-        </is>
-      </c>
-      <c r="K33" s="2" t="n">
-        <v>43581.12827546296</v>
-      </c>
-      <c r="L33" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="M33" t="n">
-        <v>6</v>
-      </c>
-      <c r="N33" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="O33" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="P33" t="inlineStr">
-        <is>
-          <t>CO</t>
-        </is>
-      </c>
-      <c r="Q33" t="inlineStr">
         <is>
           <t>C</t>
         </is>

</xml_diff>